<commit_message>
V02 : Add news functionality
</commit_message>
<xml_diff>
--- a/data/setting_2shifts.xlsx
+++ b/data/setting_2shifts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeanmichelcheumeni/RO-Optimization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeanmichelcheumeni/RO-Optimization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC7CBE86-6B80-7745-8E6B-3342020BA197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C34F03-E2F0-D34A-983C-579F2D971A1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shift" sheetId="6" r:id="rId1"/>
@@ -128,8 +128,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -140,8 +141,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準 2" xfId="1" xr:uid="{6777F17E-C139-5144-8029-B75FCC6CE2EE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -356,8 +358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8D49F4-441B-4F58-8970-D1D0BD07EB47}">
   <dimension ref="A1:DS123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:CY1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -372,304 +374,304 @@
       <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2">
+      <c r="D1" s="1">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1">
         <v>2</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>3</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="1">
         <v>4</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="1">
         <v>5</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="1">
         <v>6</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="1">
         <v>7</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="1">
         <v>8</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="1">
         <v>9</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="1">
         <v>10</v>
       </c>
-      <c r="N1" s="2">
+      <c r="N1" s="1">
         <v>11</v>
       </c>
-      <c r="O1" s="2">
+      <c r="O1" s="1">
         <v>12</v>
       </c>
-      <c r="P1" s="2">
+      <c r="P1" s="1">
         <v>13</v>
       </c>
-      <c r="Q1" s="2">
+      <c r="Q1" s="1">
         <v>14</v>
       </c>
-      <c r="R1" s="2">
+      <c r="R1" s="1">
         <v>15</v>
       </c>
-      <c r="S1" s="2">
+      <c r="S1" s="1">
         <v>16</v>
       </c>
-      <c r="T1" s="2">
+      <c r="T1" s="1">
         <v>17</v>
       </c>
-      <c r="U1" s="2">
+      <c r="U1" s="1">
         <v>18</v>
       </c>
-      <c r="V1" s="2">
+      <c r="V1" s="1">
         <v>19</v>
       </c>
-      <c r="W1" s="2">
+      <c r="W1" s="1">
         <v>20</v>
       </c>
-      <c r="X1" s="2">
+      <c r="X1" s="1">
         <v>21</v>
       </c>
-      <c r="Y1" s="2">
+      <c r="Y1" s="1">
         <v>22</v>
       </c>
-      <c r="Z1" s="2">
+      <c r="Z1" s="1">
         <v>23</v>
       </c>
-      <c r="AA1" s="2">
+      <c r="AA1" s="1">
         <v>24</v>
       </c>
-      <c r="AB1" s="2">
+      <c r="AB1" s="1">
         <v>25</v>
       </c>
-      <c r="AC1" s="2">
+      <c r="AC1" s="1">
         <v>26</v>
       </c>
-      <c r="AD1" s="2">
+      <c r="AD1" s="1">
         <v>27</v>
       </c>
-      <c r="AE1" s="2">
+      <c r="AE1" s="1">
         <v>28</v>
       </c>
-      <c r="AF1" s="2">
+      <c r="AF1" s="1">
         <v>29</v>
       </c>
-      <c r="AG1" s="2">
+      <c r="AG1" s="1">
         <v>30</v>
       </c>
-      <c r="AH1" s="2">
+      <c r="AH1" s="1">
         <v>31</v>
       </c>
-      <c r="AI1" s="2">
+      <c r="AI1" s="1">
         <v>32</v>
       </c>
-      <c r="AJ1" s="2">
+      <c r="AJ1" s="1">
         <v>33</v>
       </c>
-      <c r="AK1" s="2">
+      <c r="AK1" s="1">
         <v>34</v>
       </c>
-      <c r="AL1" s="2">
+      <c r="AL1" s="1">
         <v>35</v>
       </c>
-      <c r="AM1" s="2">
+      <c r="AM1" s="1">
         <v>36</v>
       </c>
-      <c r="AN1" s="2">
+      <c r="AN1" s="1">
         <v>37</v>
       </c>
-      <c r="AO1" s="2">
+      <c r="AO1" s="1">
         <v>38</v>
       </c>
-      <c r="AP1" s="2">
+      <c r="AP1" s="1">
         <v>39</v>
       </c>
-      <c r="AQ1" s="2">
+      <c r="AQ1" s="1">
         <v>40</v>
       </c>
-      <c r="AR1" s="2">
+      <c r="AR1" s="1">
         <v>41</v>
       </c>
-      <c r="AS1" s="2">
+      <c r="AS1" s="1">
         <v>42</v>
       </c>
-      <c r="AT1" s="2">
+      <c r="AT1" s="1">
         <v>43</v>
       </c>
-      <c r="AU1" s="2">
+      <c r="AU1" s="1">
         <v>44</v>
       </c>
-      <c r="AV1" s="2">
+      <c r="AV1" s="1">
         <v>45</v>
       </c>
-      <c r="AW1" s="2">
+      <c r="AW1" s="1">
         <v>46</v>
       </c>
-      <c r="AX1" s="2">
+      <c r="AX1" s="1">
         <v>47</v>
       </c>
-      <c r="AY1" s="2">
+      <c r="AY1" s="1">
         <v>48</v>
       </c>
-      <c r="AZ1" s="2">
+      <c r="AZ1" s="1">
         <v>49</v>
       </c>
-      <c r="BA1" s="2">
+      <c r="BA1" s="1">
         <v>50</v>
       </c>
-      <c r="BB1" s="2">
+      <c r="BB1" s="1">
         <v>51</v>
       </c>
-      <c r="BC1" s="2">
+      <c r="BC1" s="1">
         <v>52</v>
       </c>
-      <c r="BD1" s="2">
+      <c r="BD1" s="1">
         <v>53</v>
       </c>
-      <c r="BE1" s="2">
+      <c r="BE1" s="1">
         <v>54</v>
       </c>
-      <c r="BF1" s="2">
+      <c r="BF1" s="1">
         <v>55</v>
       </c>
-      <c r="BG1" s="2">
+      <c r="BG1" s="1">
         <v>56</v>
       </c>
-      <c r="BH1" s="2">
+      <c r="BH1" s="1">
         <v>57</v>
       </c>
-      <c r="BI1" s="2">
+      <c r="BI1" s="1">
         <v>58</v>
       </c>
-      <c r="BJ1" s="2">
+      <c r="BJ1" s="1">
         <v>59</v>
       </c>
-      <c r="BK1" s="2">
+      <c r="BK1" s="1">
         <v>60</v>
       </c>
-      <c r="BL1" s="2">
+      <c r="BL1" s="1">
         <v>61</v>
       </c>
-      <c r="BM1" s="2">
+      <c r="BM1" s="1">
         <v>62</v>
       </c>
-      <c r="BN1" s="2">
+      <c r="BN1" s="1">
         <v>63</v>
       </c>
-      <c r="BO1" s="2">
+      <c r="BO1" s="1">
         <v>64</v>
       </c>
-      <c r="BP1" s="2">
+      <c r="BP1" s="1">
         <v>65</v>
       </c>
-      <c r="BQ1" s="2">
+      <c r="BQ1" s="1">
         <v>66</v>
       </c>
-      <c r="BR1" s="2">
+      <c r="BR1" s="1">
         <v>67</v>
       </c>
-      <c r="BS1" s="2">
+      <c r="BS1" s="1">
         <v>68</v>
       </c>
-      <c r="BT1" s="2">
+      <c r="BT1" s="1">
         <v>69</v>
       </c>
-      <c r="BU1" s="2">
+      <c r="BU1" s="1">
         <v>70</v>
       </c>
-      <c r="BV1" s="2">
+      <c r="BV1" s="1">
         <v>71</v>
       </c>
-      <c r="BW1" s="2">
+      <c r="BW1" s="1">
         <v>72</v>
       </c>
-      <c r="BX1" s="2">
+      <c r="BX1" s="1">
         <v>73</v>
       </c>
-      <c r="BY1" s="2">
+      <c r="BY1" s="1">
         <v>74</v>
       </c>
-      <c r="BZ1" s="2">
+      <c r="BZ1" s="1">
         <v>75</v>
       </c>
-      <c r="CA1" s="2">
+      <c r="CA1" s="1">
         <v>76</v>
       </c>
-      <c r="CB1" s="2">
+      <c r="CB1" s="1">
         <v>77</v>
       </c>
-      <c r="CC1" s="2">
+      <c r="CC1" s="1">
         <v>78</v>
       </c>
-      <c r="CD1" s="2">
+      <c r="CD1" s="1">
         <v>79</v>
       </c>
-      <c r="CE1" s="2">
+      <c r="CE1" s="1">
         <v>80</v>
       </c>
-      <c r="CF1" s="2">
+      <c r="CF1" s="1">
         <v>81</v>
       </c>
-      <c r="CG1" s="2">
+      <c r="CG1" s="1">
         <v>82</v>
       </c>
-      <c r="CH1" s="2">
+      <c r="CH1" s="1">
         <v>83</v>
       </c>
-      <c r="CI1" s="2">
+      <c r="CI1" s="1">
         <v>84</v>
       </c>
-      <c r="CJ1" s="2">
+      <c r="CJ1" s="1">
         <v>85</v>
       </c>
-      <c r="CK1" s="2">
+      <c r="CK1" s="1">
         <v>86</v>
       </c>
-      <c r="CL1" s="2">
+      <c r="CL1" s="1">
         <v>87</v>
       </c>
-      <c r="CM1" s="2">
+      <c r="CM1" s="1">
         <v>88</v>
       </c>
-      <c r="CN1" s="2">
+      <c r="CN1" s="1">
         <v>89</v>
       </c>
-      <c r="CO1" s="2">
+      <c r="CO1" s="1">
         <v>90</v>
       </c>
-      <c r="CP1" s="2">
+      <c r="CP1" s="1">
         <v>91</v>
       </c>
-      <c r="CQ1" s="2">
+      <c r="CQ1" s="1">
         <v>92</v>
       </c>
-      <c r="CR1" s="2">
+      <c r="CR1" s="1">
         <v>93</v>
       </c>
-      <c r="CS1" s="2">
+      <c r="CS1" s="1">
         <v>94</v>
       </c>
-      <c r="CT1" s="2">
+      <c r="CT1" s="1">
         <v>95</v>
       </c>
-      <c r="CU1" s="2">
+      <c r="CU1" s="1">
         <v>96</v>
       </c>
-      <c r="CV1" s="2">
+      <c r="CV1" s="1">
         <v>97</v>
       </c>
-      <c r="CW1" s="2">
+      <c r="CW1" s="1">
         <v>98</v>
       </c>
-      <c r="CX1" s="2">
+      <c r="CX1" s="1">
         <v>99</v>
       </c>
-      <c r="CY1" s="2">
+      <c r="CY1" s="1">
         <v>100</v>
       </c>
     </row>
@@ -40283,7 +40285,7 @@
   <dimension ref="A1:DQ999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="CX2" sqref="CX2"/>
+      <selection activeCell="B1" sqref="B1:CW1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -43222,7 +43224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>